<commit_message>
Resulta que tocaba especificar el esquema en los permisos, ah y actualicé el CRUD, ahora es ECRUD
</commit_message>
<xml_diff>
--- a/Documentación/Matriz CRUD.xlsx
+++ b/Documentación/Matriz CRUD.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Github\BD_2025_SIMBA\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE092A7-ACB4-441A-81C9-49FF15F2E228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF4346D-E467-46A0-B61A-C2CA71381624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRUD Tablas" sheetId="2" r:id="rId1"/>
     <sheet name="CRUD Vistas" sheetId="1" r:id="rId2"/>
+    <sheet name="ECRUD Post-Procedimientos" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="64">
   <si>
     <t>Administrador</t>
   </si>
@@ -132,6 +133,87 @@
   </si>
   <si>
     <t>turno_mon</t>
+  </si>
+  <si>
+    <t>vw_Ocupacion_Diaria</t>
+  </si>
+  <si>
+    <t>vw_Ocupacion_Salas</t>
+  </si>
+  <si>
+    <t>sp_nuevaSesion</t>
+  </si>
+  <si>
+    <t>sp_cerrarSesion</t>
+  </si>
+  <si>
+    <t>sp_verSesionesActuales</t>
+  </si>
+  <si>
+    <t>sp_VerSesionesHistorial</t>
+  </si>
+  <si>
+    <t>sp_monVerEstadisticasComp</t>
+  </si>
+  <si>
+    <t>sp_monVerHistorialPc</t>
+  </si>
+  <si>
+    <t>sp_compHabilitarInhabilitar</t>
+  </si>
+  <si>
+    <t>sp_agregarComentarioSesion</t>
+  </si>
+  <si>
+    <t>sp_buscarEmpleado</t>
+  </si>
+  <si>
+    <t>sp_monNuevoEmpleado</t>
+  </si>
+  <si>
+    <t>sp_monEditarEmpleado</t>
+  </si>
+  <si>
+    <t>sp_verReservas</t>
+  </si>
+  <si>
+    <t>sp_agregarReserva</t>
+  </si>
+  <si>
+    <t>sp_cancelarReserva</t>
+  </si>
+  <si>
+    <t>sp_deshabilitarSala</t>
+  </si>
+  <si>
+    <t>sp_habilitarSala</t>
+  </si>
+  <si>
+    <t>fn_monitorLogin</t>
+  </si>
+  <si>
+    <t>sp_monitorLogout</t>
+  </si>
+  <si>
+    <t>sp_verTurnosMonitores</t>
+  </si>
+  <si>
+    <t>sp_verSupervisiones</t>
+  </si>
+  <si>
+    <t>sp_verSupervisados</t>
+  </si>
+  <si>
+    <t>sp_adminLogin</t>
+  </si>
+  <si>
+    <t>sp_verTurnosAdmins</t>
+  </si>
+  <si>
+    <t>sp_adminLogout</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -167,7 +249,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -329,11 +411,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,6 +579,78 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,7 +939,7 @@
   </sheetPr>
   <dimension ref="A2:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -840,7 +1111,7 @@
   <dimension ref="A2:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1035,4 +1306,341 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD35FF66-8279-4F7B-BE61-D5699D8F61B2}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A2:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.21875" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="37"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="33"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="36"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="34"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="32"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="33"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="33"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="33"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="33"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="36"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="32"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="33"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="33"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" s="33"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="33"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="45"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="45"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="48"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="49"/>
+      <c r="C22" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="51"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="46"/>
+      <c r="C23" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D23" s="48"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="50"/>
+      <c r="D24" s="51"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="43"/>
+      <c r="D25" s="45"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="47"/>
+      <c r="D26" s="48"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="50"/>
+      <c r="D27" s="51"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="43"/>
+      <c r="D28" s="45"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="47"/>
+      <c r="D29" s="48"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>